<commit_message>
new - 更新 3.12 中签率
</commit_message>
<xml_diff>
--- a/investment/new-stock.xlsx
+++ b/investment/new-stock.xlsx
@@ -471,6 +471,15 @@
     <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,15 +497,6 @@
     </xf>
     <xf numFmtId="7" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,7 +795,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -892,10 +892,10 @@
         <f>E2*F2</f>
         <v>172425</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2" s="27">
         <v>6.6E-3</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="28">
         <f>I2*G2</f>
         <v>9.9000000000000005E-2</v>
       </c>
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="34"/>
+      <c r="J3" s="28"/>
       <c r="L3" s="21" t="s">
         <v>51</v>
       </c>
@@ -996,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="34"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="10" t="s">
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="34"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="10" t="s">
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="34"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="8" t="s">
@@ -1079,11 +1079,11 @@
         <f t="shared" si="1"/>
         <v>111760</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="29">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="J7" s="34">
-        <f t="shared" ref="J3:J7" si="2">I7*G7</f>
+      <c r="J7" s="28">
+        <f t="shared" ref="J7:J12" si="2">I7*G7</f>
         <v>9.1200000000000003E-2</v>
       </c>
     </row>
@@ -1112,8 +1112,13 @@
         <f t="shared" si="1"/>
         <v>60690</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="I8" s="29">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="J8" s="28">
+        <f t="shared" si="2"/>
+        <v>5.7799999999999997E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:17" s="3" customFormat="1">
       <c r="A9" s="8" t="s">
@@ -1140,8 +1145,13 @@
         <f t="shared" si="1"/>
         <v>127260</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="29">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="J9" s="28">
+        <f t="shared" si="2"/>
+        <v>7.6800000000000007E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1">
       <c r="A10" s="8" t="s">
@@ -1168,8 +1178,13 @@
         <f t="shared" si="1"/>
         <v>57800</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="I10" s="29">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="J10" s="28">
+        <f t="shared" si="2"/>
+        <v>6.6299999999999998E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:17" s="3" customFormat="1">
       <c r="A11" s="8" t="s">
@@ -1196,8 +1211,13 @@
         <f t="shared" si="1"/>
         <v>201900</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="I11" s="29">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="J11" s="28">
+        <f t="shared" si="2"/>
+        <v>0.10199999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1">
       <c r="A12" s="8" t="s">
@@ -1224,8 +1244,13 @@
         <f t="shared" si="1"/>
         <v>127120</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="I12" s="29">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="J12" s="28">
+        <f t="shared" si="2"/>
+        <v>0.11840000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:17" s="6" customFormat="1">
       <c r="A13" s="11" t="s">
@@ -1398,21 +1423,21 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33">
         <f>SUM(H2:H18)</f>
         <v>1036315</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="18"/>

</xml_diff>